<commit_message>
fix 28 nov 2023
</commit_message>
<xml_diff>
--- a/studentExtracurricular.xlsx
+++ b/studentExtracurricular.xlsx
@@ -37,139 +37,136 @@
     <t>nisn</t>
   </si>
   <si>
-    <t>CAMELLIA RAHMA ZAHRANI</t>
-  </si>
-  <si>
-    <t>Perempuan</t>
-  </si>
-  <si>
     <t>ABDULLAH AZZAM BASYIR</t>
   </si>
   <si>
-    <t>Laki-laki</t>
+    <t>laki-laki</t>
+  </si>
+  <si>
+    <t>AWANSYAH HERLAS WICAKSONO</t>
+  </si>
+  <si>
+    <t>BINTANG ADITYA PUTRA PERDANA</t>
+  </si>
+  <si>
+    <t>CAMELIA RAHMA ZAHRANI</t>
+  </si>
+  <si>
+    <t>perempuan</t>
+  </si>
+  <si>
+    <t>CANTIKA PUTRI SALSABILA</t>
   </si>
   <si>
     <t>DAFINA AFILIA RAIHANAH</t>
   </si>
   <si>
+    <t>FATHIYA AILEEN FIYO MAHARANI</t>
+  </si>
+  <si>
     <t>HANIFAH MAJIDA</t>
   </si>
   <si>
+    <t>ISVARA LASHIRA QUANANDI</t>
+  </si>
+  <si>
+    <t>KEISHA LIONA JERLYN ADE</t>
+  </si>
+  <si>
+    <t>MUHAMMAD ALI ZAINAL ABIDIN</t>
+  </si>
+  <si>
+    <t>MUHAMMAD KAHFI SURYA PRATAMA</t>
+  </si>
+  <si>
+    <t>MUHAMMAD ZAYD ALTEZZA</t>
+  </si>
+  <si>
+    <t>NADIA YASMIN SAPUTRI</t>
+  </si>
+  <si>
+    <t>NUHA HUSNI GHANIM</t>
+  </si>
+  <si>
     <t>RANIA PUTRI RAMADHANI</t>
   </si>
   <si>
-    <t>BINTANG ADITYA PUTRA PERDANA</t>
+    <t>RIZQA THALITA AYUDIA MAKKAH</t>
+  </si>
+  <si>
+    <t>VALLEANDINO AR SAKHA ARSENIO</t>
   </si>
   <si>
     <t>VIGO REYNANDRA GUNAWAN</t>
   </si>
   <si>
-    <t>MUHAMMAD ZAYD ALTEZZA</t>
-  </si>
-  <si>
-    <t>MUHAMMAD ALI ZAINAL ABIDIN</t>
-  </si>
-  <si>
-    <t>NUHA HUSNI GHANIM</t>
-  </si>
-  <si>
-    <t>VALLEANDINO AR SAKHA ARSENIO</t>
-  </si>
-  <si>
-    <t>AWANSYAH HERLAS WICAKSONO</t>
-  </si>
-  <si>
-    <t>FATHIYA AILEEN FIYO MAHARANI</t>
-  </si>
-  <si>
-    <t>NADIAH YASMIN SAPUTRI</t>
-  </si>
-  <si>
-    <t>RIZQA THALITA AYUDIA MAKKAH</t>
-  </si>
-  <si>
-    <t>ISVARA LASHIRA QUANANDI</t>
-  </si>
-  <si>
-    <t>KEISHA LIONA JESLYN ADELICIA</t>
-  </si>
-  <si>
-    <t>CANTIKA PUTRI SALSABILA</t>
-  </si>
-  <si>
-    <t>MUHAMMAD KAHFI SURYA PRATAMA</t>
-  </si>
-  <si>
     <t>ALDIANO GARDIAN PUTRANSYAH</t>
   </si>
   <si>
+    <t>AINANNISA SUHARTONO</t>
+  </si>
+  <si>
+    <t>AISYAH AIDA NURVARISHA</t>
+  </si>
+  <si>
+    <t>ALINE SYAFIRA PUTRI</t>
+  </si>
+  <si>
+    <t>AMANDA SHAFIRA KHAIRUNISA</t>
+  </si>
+  <si>
+    <t>AMANY HAFID THALIB</t>
+  </si>
+  <si>
+    <t>BELVANIA NASYTA CALIEF</t>
+  </si>
+  <si>
     <t>HERJUNO FACHTUROHMI</t>
   </si>
   <si>
-    <t>AISYAH AIDA NURVARISHA</t>
-  </si>
-  <si>
-    <t>ALINE SYARIFA PUTRI</t>
-  </si>
-  <si>
-    <t>KAYLA NUR RAMADHANI</t>
+    <t>KAYLA NUR RAMADANI</t>
+  </si>
+  <si>
+    <t>MUKHAMMAD YUSUF ALFARIDZI</t>
   </si>
   <si>
     <t>NAURA FIZA SALSABILA</t>
   </si>
   <si>
-    <t>MUKHAMMAD YUSUF ALFARIDZI</t>
-  </si>
-  <si>
-    <t>AMANY HAFID THALIB</t>
-  </si>
-  <si>
-    <t>BELVANIA NASYITA CALIEF</t>
-  </si>
-  <si>
-    <t>AINANNISA SUHARTONO</t>
-  </si>
-  <si>
-    <t>ZAHIDA RAHMANIA AZ-ZAHRA</t>
-  </si>
-  <si>
-    <t>AMANDA SHAFIRA KHAIRUNISA</t>
-  </si>
-  <si>
-    <t>SANINAH HUMMAIRAH FARUK</t>
+    <t>SANINA HUMAIRAH FARUK</t>
+  </si>
+  <si>
+    <t>ZAHIDA RAHMANIA</t>
   </si>
   <si>
     <t>MUHAMMAD FATHIR ALKINDI</t>
   </si>
   <si>
-    <t>MUHAMMAD ATHAR AL RAMADHAN</t>
-  </si>
-  <si>
     <t>ABIMANYU YUSVIANANDA ALFATIH PRADISTA</t>
   </si>
   <si>
+    <t>AKHMAD FARZANA AMRAN SISWANTO</t>
+  </si>
+  <si>
+    <t>ALLEGRO julyAN VICKY SAPUTRA</t>
+  </si>
+  <si>
+    <t>AXEEL ATHALLAH AL HAFIZH</t>
+  </si>
+  <si>
+    <t>DZAKI HAMDAN PRATAMA</t>
+  </si>
+  <si>
+    <t>I WAYAN MERVLO SHAFWAN DNAVA</t>
+  </si>
+  <si>
+    <t>INARA CAHYA PRAMESTI</t>
+  </si>
+  <si>
     <t>KAYLA CALISTA SAPUTRA</t>
   </si>
   <si>
-    <t>AXEEL ATHALLAH AL HAFIZH</t>
-  </si>
-  <si>
-    <t>ALLEGRO JULIAN VICKY SAPUTRA</t>
-  </si>
-  <si>
-    <t>ZHAFRAN SULTHANA THORSYAHDIKA</t>
-  </si>
-  <si>
-    <t>AKHMAD FARZANA AMRAN SISWANTO</t>
-  </si>
-  <si>
-    <t>I WAYAN MERVLO SHAFWAN DNAVA</t>
-  </si>
-  <si>
-    <t>INARA CAHYA PRAMESTI</t>
-  </si>
-  <si>
-    <t>DZAKI HAMDAN PRATAMA</t>
+    <t>MUHAMMAD ATHAR AL RAHMAN</t>
   </si>
   <si>
     <t>MUHAMMAD RAZIQ VIRENDRA AHSAN</t>
@@ -181,202 +178,205 @@
     <t>ZAHIDA NUR AMELIA</t>
   </si>
   <si>
+    <t>ZHAFRAN SULTANA THORSYAHDIKA</t>
+  </si>
+  <si>
+    <t>AHMAD CELLO OBIANZ</t>
+  </si>
+  <si>
+    <t>AISYAH ELMIRA PUTRI WIJAYA</t>
+  </si>
+  <si>
+    <t>AKILA FITRIA RAMADAN</t>
+  </si>
+  <si>
+    <t>ALVINA SUCI RAMADHANI</t>
+  </si>
+  <si>
+    <t>AQILA HASNA KAMILA</t>
+  </si>
+  <si>
+    <t>AZKA GIOVANI SETIAWAN</t>
+  </si>
+  <si>
+    <t>AZZAM BHARIQ FAIZULLAH</t>
+  </si>
+  <si>
+    <t>FARID IRFAN MAULANA HAKIM</t>
+  </si>
+  <si>
+    <t>HAMIM LANANDER ALIBUKHORI</t>
+  </si>
+  <si>
+    <t>IBRAHIM ZHAFFRAN NEELEMAN</t>
+  </si>
+  <si>
+    <t>JAYLANI ABDILLAH</t>
+  </si>
+  <si>
+    <t>MUHAMMAD AKBAR MAULANA</t>
+  </si>
+  <si>
+    <t>NARRATAMA ERABBANI ALIFIANDRA</t>
+  </si>
+  <si>
+    <t>PRAMUDYA ATHALLAH ARFA</t>
+  </si>
+  <si>
+    <t>RADELLA SYANUM YOSITA ALI</t>
+  </si>
+  <si>
+    <t>RAISA SISCA RAMADHAN</t>
+  </si>
+  <si>
+    <t>RIDHO RAMADHAN</t>
+  </si>
+  <si>
+    <t>TOTTI ALTAIR REVANO</t>
+  </si>
+  <si>
+    <t>ZIVIARA ASKANA SHAKI</t>
+  </si>
+  <si>
     <t>FAIQA AZZAHRA</t>
   </si>
   <si>
-    <t>MUHAMMAD AKBAR MAULANA</t>
-  </si>
-  <si>
-    <t>ALVINA SUCI RAMADHANI</t>
-  </si>
-  <si>
-    <t>AHMAD CELLO OBIANZ</t>
-  </si>
-  <si>
-    <t>RIDHO RAMADHAN</t>
-  </si>
-  <si>
-    <t>AKILA FITRIA RAMADHAN</t>
-  </si>
-  <si>
-    <t>IBRAHIM ZHAFFRAN NEELEMAN</t>
-  </si>
-  <si>
-    <t>HAMIM LANANDER  ALBUKHORI</t>
-  </si>
-  <si>
-    <t>RAISA SISCA RAMADHAN</t>
-  </si>
-  <si>
-    <t>PRAMUDYA ATHALLAH ARFA</t>
-  </si>
-  <si>
-    <t>NARRATAMA ERABBANI ALIFIANDRA</t>
-  </si>
-  <si>
-    <t>AQILA HASNA KAMILA</t>
-  </si>
-  <si>
-    <t>RADELLA SYANUM YOSITA ALI</t>
-  </si>
-  <si>
-    <t>AISYAH ELMIRA PUTRI WIJAYA</t>
-  </si>
-  <si>
-    <t>FARID IRFAN MAULANA HAKIM</t>
-  </si>
-  <si>
-    <t>JAYLANI ABDILLAH</t>
-  </si>
-  <si>
-    <t>AZZAM BHARIQ FAIZHULLAH</t>
-  </si>
-  <si>
-    <t>ZIVIARA ASKANA SAKHI</t>
-  </si>
-  <si>
-    <t>AZKA GIOVANI SETIAWAN</t>
-  </si>
-  <si>
-    <t>TOTTI ALTAIR REVANO</t>
+    <t>AKHTAR IRSYAD AZIZI</t>
+  </si>
+  <si>
+    <t>ALMIRA PRAMESWARI NARENDRA BUWANA</t>
+  </si>
+  <si>
+    <t>ANANTA RHEZKY SANJAYA</t>
+  </si>
+  <si>
+    <t>AZIDAN REGINALD LUBIS</t>
   </si>
   <si>
     <t>DASTAN ALFIAN FADHILAH</t>
   </si>
   <si>
-    <t>ANANTA RHEZKY SANJAYA</t>
+    <t>DEHAN BRAHMA ALVARO</t>
+  </si>
+  <si>
+    <t>FATIMAH BASMA</t>
   </si>
   <si>
     <t>KEANO ADISAPUTRA HERMAWAN</t>
   </si>
   <si>
-    <t>FATIMAH BASMA</t>
-  </si>
-  <si>
-    <t>ALMIRA PRAMESWARI NARENDRA BUWANA</t>
-  </si>
-  <si>
-    <t>AKHTAR IRSYAD A'ZIZI</t>
+    <t>KEISHA MAHRA SALSABILLA</t>
+  </si>
+  <si>
+    <t>LAMIA HUSNI GHANIM</t>
   </si>
   <si>
     <t>MAZAYA AISYAH SETIAWAN</t>
   </si>
   <si>
-    <t>NIKO ALFATIH</t>
+    <t>MUHAMMAD HANIIF AKHTAR ROSIKH</t>
+  </si>
+  <si>
+    <t>MUHAMMAD RAFA LUKMANSYAH</t>
+  </si>
+  <si>
+    <t>NIKO AL FATIH</t>
+  </si>
+  <si>
+    <t>NOVIANA NAIMA MARDHATIN</t>
+  </si>
+  <si>
+    <t>RAJA RIZKY IRAWAN</t>
   </si>
   <si>
     <t>RICKY HAIDAR FAHEEM</t>
   </si>
   <si>
-    <t>NOVIANA NAIMA MARDHATIN</t>
-  </si>
-  <si>
-    <t>KEISHA MAHRA SALSABILLA</t>
-  </si>
-  <si>
-    <t>DEHAN BRAMA ALVARO</t>
-  </si>
-  <si>
     <t>SAFINA FIRLY ALAMRI</t>
   </si>
   <si>
-    <t>AZIDAN REGINALD LUBIS</t>
-  </si>
-  <si>
-    <t>RAJA RIZKY IRAWAN</t>
-  </si>
-  <si>
-    <t>LAMIA HUSNI GHANIM</t>
-  </si>
-  <si>
-    <t>MUHAMMAD RAFA LUKMANSYAH</t>
-  </si>
-  <si>
-    <t>MUHAMMAD HANIIF AKHTAR ROSIKH</t>
-  </si>
-  <si>
     <t>HUMAIRA PUTRI EKASANDHI</t>
   </si>
   <si>
+    <t>ACHMAD KURNIAWAN</t>
+  </si>
+  <si>
+    <t>ACHMADIKA HUSYAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJI SYAHPUTRA </t>
+  </si>
+  <si>
+    <t>ALIYYA AZZAHRA PUTRI BASKURI ACHMAD</t>
+  </si>
+  <si>
+    <t>ANANTAVIRYA SATWIKA PUTRA</t>
+  </si>
+  <si>
+    <t>ARHABURRIZQY ZAIDAN ATHALLAH</t>
+  </si>
+  <si>
+    <t>ARKAN KENZIE PRASETYA</t>
+  </si>
+  <si>
+    <t>ATHA'ILLAH NAFIS RAYKHAN</t>
+  </si>
+  <si>
+    <t>ATHAYA RAYYAN KEANU PRIBADI</t>
+  </si>
+  <si>
+    <t>AWAN SWARGA PANJI ASMORO</t>
+  </si>
+  <si>
+    <t>DANISH ATHAILLAH PRADIPTA</t>
+  </si>
+  <si>
+    <t>EL-MAGHRIBI KALLE NALENDRA</t>
+  </si>
+  <si>
+    <t>FAIZAL NUR IKHSAN</t>
+  </si>
+  <si>
+    <t>HARVANTYO ABBAD ZIZOU SANTOSO</t>
+  </si>
+  <si>
+    <t>KAMAY KEGY ANINDITA</t>
+  </si>
+  <si>
+    <t>MUHAMMAD AL FATIH</t>
+  </si>
+  <si>
+    <t>MUHAMMAD AQIL AZIZI</t>
+  </si>
+  <si>
+    <t>MUHAMMAD FAISAL AL FAKHRISI</t>
+  </si>
+  <si>
+    <t>MUHAMMAD FAIZ NUR HAFIDZ</t>
+  </si>
+  <si>
+    <t>MUHAMMAD NABIL ARSYAD</t>
+  </si>
+  <si>
+    <t>MUHAMMAD RAQI AZAM MAULANA</t>
+  </si>
+  <si>
     <t>MUHAMMAD ZHAFIR FERDIANSYAH ALTHAF</t>
   </si>
   <si>
-    <t>ATHA'ILAH NAFIS RAYKHAN</t>
-  </si>
-  <si>
-    <t>MUHAMMAD NABIL ARSYAD</t>
-  </si>
-  <si>
-    <t>DANISH ATHAILLAH PRADIPTA</t>
-  </si>
-  <si>
-    <t>MUHAMMAD FAIZ NUR HAFIDZ</t>
-  </si>
-  <si>
-    <t>ACHMAD KURNIAWAN</t>
-  </si>
-  <si>
-    <t>MUHAMMAD FAISAL AL FAKHRISI</t>
+    <t>MUHAMMAD ZIGGY SAVERIO LATIF</t>
+  </si>
+  <si>
+    <t>RAFA ANDIKA ABIYU</t>
+  </si>
+  <si>
+    <t>RAHMAH FAZILA PUTRI</t>
   </si>
   <si>
     <t>RAJENDRA ARYA BAYU YUDHISTIRA</t>
   </si>
   <si>
-    <t>MUHAMMAD RAQI AZAM MAULANA</t>
-  </si>
-  <si>
-    <t>ATHAYA RAYYAN KEANU PRIBADI</t>
-  </si>
-  <si>
-    <t>HARVANTYO ABBAD ZIZOU SANTOSO</t>
-  </si>
-  <si>
-    <t>EL MAGHRIBI KALLE NALENDRA</t>
-  </si>
-  <si>
-    <t>ARKAN KENZIE PRASETYA</t>
-  </si>
-  <si>
-    <t>AJI SYAPUTRA</t>
-  </si>
-  <si>
-    <t>ACHMADIKA HUSYAIN</t>
-  </si>
-  <si>
     <t>SATRIA WANAMANDALA GINTING</t>
-  </si>
-  <si>
-    <t>MUHAMMAD ZIGGY SAVERIO CALIEF</t>
-  </si>
-  <si>
-    <t>FAIZAL NUR IKHSAN</t>
-  </si>
-  <si>
-    <t>MUHAMMAD AQIL AZIZI</t>
-  </si>
-  <si>
-    <t>RAHMAH FAZILA PUTRI</t>
-  </si>
-  <si>
-    <t>ALLIYA AZZAHRA PUTRI BASKURI ACHMAD</t>
-  </si>
-  <si>
-    <t>RAFA ANDIKA ABIYU</t>
-  </si>
-  <si>
-    <t>AWAN SWARGA PANJI ASMORO</t>
-  </si>
-  <si>
-    <t>ARHABURRIZQI ZAIDAN ATHALLAH</t>
-  </si>
-  <si>
-    <t>KAMAY KEGY ANINDITA</t>
-  </si>
-  <si>
-    <t>MUHAMMAD ALFATIH</t>
-  </si>
-  <si>
-    <t>ANANTAVIRYA SATWIKA PUTRA</t>
   </si>
   <si>
     <t>TALITHA PUTRI PAMBAYUN</t>
@@ -746,7 +746,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -800,6 +800,1022 @@
       </c>
       <c r="B6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>5</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <v>5</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88">
+        <v>5</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98">
+        <v>5</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99">
+        <v>5</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101">
+        <v>5</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102">
+        <v>5</v>
+      </c>
+      <c r="B102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103">
+        <v>5</v>
+      </c>
+      <c r="B103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104">
+        <v>5</v>
+      </c>
+      <c r="B104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105">
+        <v>5</v>
+      </c>
+      <c r="B105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106">
+        <v>5</v>
+      </c>
+      <c r="B106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107">
+        <v>5</v>
+      </c>
+      <c r="B107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108">
+        <v>5</v>
+      </c>
+      <c r="B108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109">
+        <v>5</v>
+      </c>
+      <c r="B109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110">
+        <v>5</v>
+      </c>
+      <c r="B110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111">
+        <v>5</v>
+      </c>
+      <c r="B111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112">
+        <v>5</v>
+      </c>
+      <c r="B112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113">
+        <v>5</v>
+      </c>
+      <c r="B113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114">
+        <v>5</v>
+      </c>
+      <c r="B114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115">
+        <v>6</v>
+      </c>
+      <c r="B115">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116">
+        <v>6</v>
+      </c>
+      <c r="B116">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117">
+        <v>6</v>
+      </c>
+      <c r="B117">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118">
+        <v>6</v>
+      </c>
+      <c r="B118">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119">
+        <v>6</v>
+      </c>
+      <c r="B119">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120">
+        <v>6</v>
+      </c>
+      <c r="B120">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121">
+        <v>6</v>
+      </c>
+      <c r="B121">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122">
+        <v>6</v>
+      </c>
+      <c r="B122">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123">
+        <v>6</v>
+      </c>
+      <c r="B123">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124">
+        <v>6</v>
+      </c>
+      <c r="B124">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125">
+        <v>6</v>
+      </c>
+      <c r="B125">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126">
+        <v>6</v>
+      </c>
+      <c r="B126">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127">
+        <v>6</v>
+      </c>
+      <c r="B127">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128">
+        <v>6</v>
+      </c>
+      <c r="B128">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129">
+        <v>6</v>
+      </c>
+      <c r="B129">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130">
+        <v>6</v>
+      </c>
+      <c r="B130">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131">
+        <v>6</v>
+      </c>
+      <c r="B131">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132">
+        <v>6</v>
+      </c>
+      <c r="B132">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133">
+        <v>6</v>
+      </c>
+      <c r="B133">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -859,10 +1875,10 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>2023001</v>
+        <v>230001</v>
       </c>
       <c r="E2">
-        <v>3162867827</v>
+        <v>230001</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -873,13 +1889,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>2023002</v>
+        <v>230002</v>
       </c>
       <c r="E3">
-        <v>3166534301</v>
+        <v>230002</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -887,16 +1903,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4">
-        <v>2023003</v>
+        <v>230003</v>
       </c>
       <c r="E4">
-        <v>3169744676</v>
+        <v>230003</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -904,16 +1920,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>2023004</v>
+        <v>230004</v>
       </c>
       <c r="E5">
-        <v>3160135852</v>
+        <v>230004</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -924,13 +1940,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>2023005</v>
+        <v>230005</v>
       </c>
       <c r="E6">
-        <v>3165517173</v>
+        <v>230005</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -941,13 +1957,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>2023006</v>
+        <v>230006</v>
       </c>
       <c r="E7">
-        <v>3169439398</v>
+        <v>230006</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -958,13 +1974,13 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>2023007</v>
+        <v>230007</v>
       </c>
       <c r="E8">
-        <v>3166698294</v>
+        <v>230007</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -975,13 +1991,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>2023008</v>
+        <v>230008</v>
       </c>
       <c r="E9">
-        <v>163759489</v>
+        <v>230008</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -992,13 +2008,13 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>2023009</v>
+        <v>230009</v>
       </c>
       <c r="E10">
-        <v>164202109</v>
+        <v>230009</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1009,13 +2025,13 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>2023010</v>
+        <v>230010</v>
       </c>
       <c r="E11">
-        <v>3174954599</v>
+        <v>230010</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1026,13 +2042,13 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12">
-        <v>2023011</v>
+        <v>230011</v>
       </c>
       <c r="E12">
-        <v>167123418</v>
+        <v>230011</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1043,13 +2059,13 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>2023012</v>
+        <v>230012</v>
       </c>
       <c r="E13">
-        <v>163493366</v>
+        <v>230012</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1063,10 +2079,10 @@
         <v>7</v>
       </c>
       <c r="D14">
-        <v>2023013</v>
+        <v>230013</v>
       </c>
       <c r="E14">
-        <v>3164269918</v>
+        <v>230013</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1077,13 +2093,13 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>2023014</v>
+        <v>230014</v>
       </c>
       <c r="E15">
-        <v>3175825294</v>
+        <v>230014</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1094,13 +2110,13 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D16">
-        <v>2023015</v>
+        <v>230015</v>
       </c>
       <c r="E16">
-        <v>3160022135</v>
+        <v>230015</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1111,13 +2127,13 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D17">
-        <v>2023016</v>
+        <v>230016</v>
       </c>
       <c r="E17">
-        <v>3162752117</v>
+        <v>230016</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1128,13 +2144,13 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>2023017</v>
+        <v>230017</v>
       </c>
       <c r="E18">
-        <v>3167280470</v>
+        <v>230017</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1148,10 +2164,10 @@
         <v>7</v>
       </c>
       <c r="D19">
-        <v>2023018</v>
+        <v>230018</v>
       </c>
       <c r="E19">
-        <v>3168436629</v>
+        <v>230018</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1162,13 +2178,13 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D20">
-        <v>2023019</v>
+        <v>230019</v>
       </c>
       <c r="E20">
-        <v>3175576407</v>
+        <v>230019</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1179,13 +2195,13 @@
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>2023020</v>
+        <v>230020</v>
       </c>
       <c r="E21">
-        <v>3162677659</v>
+        <v>230020</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1196,13 +2212,13 @@
         <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>2022001</v>
+        <v>220001</v>
       </c>
       <c r="E22">
-        <v>3150474347</v>
+        <v>220001</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1213,13 +2229,13 @@
         <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>2022002</v>
+        <v>220002</v>
       </c>
       <c r="E23">
-        <v>3157516338</v>
+        <v>220002</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1230,13 +2246,13 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D24">
-        <v>2022003</v>
+        <v>220003</v>
       </c>
       <c r="E24">
-        <v>3161418035</v>
+        <v>220003</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1247,13 +2263,13 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D25">
-        <v>2022004</v>
+        <v>220004</v>
       </c>
       <c r="E25">
-        <v>3150018552</v>
+        <v>220004</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1264,13 +2280,13 @@
         <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26">
-        <v>2022005</v>
+        <v>220005</v>
       </c>
       <c r="E26">
-        <v>3153736392</v>
+        <v>220005</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1281,13 +2297,13 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D27">
-        <v>2022006</v>
+        <v>220006</v>
       </c>
       <c r="E27">
-        <v>3169677068</v>
+        <v>220006</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1301,10 +2317,10 @@
         <v>7</v>
       </c>
       <c r="D28">
-        <v>2022007</v>
+        <v>220007</v>
       </c>
       <c r="E28">
-        <v>3161571800</v>
+        <v>220007</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1315,13 +2331,13 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D29">
-        <v>2022008</v>
+        <v>220008</v>
       </c>
       <c r="E29">
-        <v>3153364328</v>
+        <v>220008</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1335,10 +2351,10 @@
         <v>7</v>
       </c>
       <c r="D30">
-        <v>2022009</v>
+        <v>220009</v>
       </c>
       <c r="E30">
-        <v>3157982766</v>
+        <v>220009</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1349,13 +2365,13 @@
         <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D31">
-        <v>2022010</v>
+        <v>220010</v>
       </c>
       <c r="E31">
-        <v>3158192494</v>
+        <v>220010</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1366,13 +2382,13 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>2022011</v>
+        <v>220011</v>
       </c>
       <c r="E32">
-        <v>3145959991</v>
+        <v>220011</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1383,13 +2399,13 @@
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D33">
-        <v>2022012</v>
+        <v>220012</v>
       </c>
       <c r="E33">
-        <v>3160005533</v>
+        <v>220012</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1403,10 +2419,10 @@
         <v>7</v>
       </c>
       <c r="D34">
-        <v>2022013</v>
+        <v>230021</v>
       </c>
       <c r="E34">
-        <v>3159086312</v>
+        <v>230021</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1420,10 +2436,10 @@
         <v>7</v>
       </c>
       <c r="D35">
-        <v>2021001</v>
+        <v>210001</v>
       </c>
       <c r="E35">
-        <v>3142036620</v>
+        <v>210001</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1437,10 +2453,10 @@
         <v>7</v>
       </c>
       <c r="D36">
-        <v>2021002</v>
+        <v>210002</v>
       </c>
       <c r="E36">
-        <v>3145335843</v>
+        <v>210002</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1454,10 +2470,10 @@
         <v>7</v>
       </c>
       <c r="D37">
-        <v>2021003</v>
+        <v>210003</v>
       </c>
       <c r="E37">
-        <v>3143068726</v>
+        <v>210003</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1471,10 +2487,10 @@
         <v>7</v>
       </c>
       <c r="D38">
-        <v>2021004</v>
+        <v>210004</v>
       </c>
       <c r="E38">
-        <v>3147892084</v>
+        <v>210004</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1488,10 +2504,10 @@
         <v>7</v>
       </c>
       <c r="D39">
-        <v>2021005</v>
+        <v>210005</v>
       </c>
       <c r="E39">
-        <v>3141564731</v>
+        <v>210005</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1505,10 +2521,10 @@
         <v>7</v>
       </c>
       <c r="D40">
-        <v>2021006</v>
+        <v>210006</v>
       </c>
       <c r="E40">
-        <v>3148578656</v>
+        <v>210006</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1519,13 +2535,13 @@
         <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D41">
-        <v>2021007</v>
+        <v>210007</v>
       </c>
       <c r="E41">
-        <v>3149166654</v>
+        <v>210007</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1536,13 +2552,13 @@
         <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D42">
-        <v>2021008</v>
+        <v>210008</v>
       </c>
       <c r="E42">
-        <v>3153314805</v>
+        <v>210008</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1556,10 +2572,10 @@
         <v>7</v>
       </c>
       <c r="D43">
-        <v>2021009</v>
+        <v>210009</v>
       </c>
       <c r="E43">
-        <v>131128459</v>
+        <v>210009</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1573,10 +2589,10 @@
         <v>7</v>
       </c>
       <c r="D44">
-        <v>2021010</v>
+        <v>210010</v>
       </c>
       <c r="E44">
-        <v>142318029</v>
+        <v>210010</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1587,13 +2603,13 @@
         <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D45">
-        <v>2021011</v>
+        <v>210011</v>
       </c>
       <c r="E45">
-        <v>159142173</v>
+        <v>210011</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1604,13 +2620,13 @@
         <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D46">
-        <v>2021012</v>
+        <v>210012</v>
       </c>
       <c r="E46">
-        <v>3147155548</v>
+        <v>210012</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1624,10 +2640,10 @@
         <v>7</v>
       </c>
       <c r="D47">
-        <v>2021013</v>
+        <v>210013</v>
       </c>
       <c r="E47">
-        <v>147697493</v>
+        <v>210013</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1641,10 +2657,10 @@
         <v>7</v>
       </c>
       <c r="D48">
-        <v>2020001</v>
+        <v>200001</v>
       </c>
       <c r="E48">
-        <v>134554725</v>
+        <v>200001</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1655,13 +2671,13 @@
         <v>55</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D49">
-        <v>2020002</v>
+        <v>200002</v>
       </c>
       <c r="E49">
-        <v>3135392621</v>
+        <v>200002</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1672,13 +2688,13 @@
         <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D50">
-        <v>2020003</v>
+        <v>200003</v>
       </c>
       <c r="E50">
-        <v>3147112410</v>
+        <v>200003</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1689,13 +2705,13 @@
         <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D51">
-        <v>2020004</v>
+        <v>200004</v>
       </c>
       <c r="E51">
-        <v>3138974794</v>
+        <v>200004</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1706,13 +2722,13 @@
         <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D52">
-        <v>2020005</v>
+        <v>200005</v>
       </c>
       <c r="E52">
-        <v>3142912632</v>
+        <v>200005</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1726,10 +2742,10 @@
         <v>7</v>
       </c>
       <c r="D53">
-        <v>2020006</v>
+        <v>200006</v>
       </c>
       <c r="E53">
-        <v>3144519865</v>
+        <v>200006</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1743,10 +2759,10 @@
         <v>7</v>
       </c>
       <c r="D54">
-        <v>2020007</v>
+        <v>200007</v>
       </c>
       <c r="E54">
-        <v>134530554</v>
+        <v>200007</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1760,10 +2776,10 @@
         <v>7</v>
       </c>
       <c r="D55">
-        <v>2020008</v>
+        <v>200008</v>
       </c>
       <c r="E55">
-        <v>132109062</v>
+        <v>200008</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1777,10 +2793,10 @@
         <v>7</v>
       </c>
       <c r="D56">
-        <v>2020009</v>
+        <v>200009</v>
       </c>
       <c r="E56">
-        <v>147852141</v>
+        <v>200009</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1794,10 +2810,10 @@
         <v>7</v>
       </c>
       <c r="D57">
-        <v>2020010</v>
+        <v>200010</v>
       </c>
       <c r="E57">
-        <v>3131011500</v>
+        <v>200010</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1811,10 +2827,10 @@
         <v>7</v>
       </c>
       <c r="D58">
-        <v>2020011</v>
+        <v>200011</v>
       </c>
       <c r="E58">
-        <v>3138301623</v>
+        <v>200011</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1828,10 +2844,10 @@
         <v>7</v>
       </c>
       <c r="D59">
-        <v>2020012</v>
+        <v>200012</v>
       </c>
       <c r="E59">
-        <v>3137909230</v>
+        <v>200012</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1845,10 +2861,10 @@
         <v>7</v>
       </c>
       <c r="D60">
-        <v>2020013</v>
+        <v>200013</v>
       </c>
       <c r="E60">
-        <v>3144510084</v>
+        <v>200013</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1862,10 +2878,10 @@
         <v>7</v>
       </c>
       <c r="D61">
-        <v>2020014</v>
+        <v>200014</v>
       </c>
       <c r="E61">
-        <v>3135733319</v>
+        <v>200014</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1876,13 +2892,13 @@
         <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D62">
-        <v>2020015</v>
+        <v>200015</v>
       </c>
       <c r="E62">
-        <v>3136043703</v>
+        <v>200015</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1893,13 +2909,13 @@
         <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D63">
-        <v>2020016</v>
+        <v>200016</v>
       </c>
       <c r="E63">
-        <v>3139785732</v>
+        <v>200016</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1913,10 +2929,10 @@
         <v>7</v>
       </c>
       <c r="D64">
-        <v>2020017</v>
+        <v>200017</v>
       </c>
       <c r="E64">
-        <v>3130950096</v>
+        <v>200017</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1930,10 +2946,10 @@
         <v>7</v>
       </c>
       <c r="D65">
-        <v>2020018</v>
+        <v>200018</v>
       </c>
       <c r="E65">
-        <v>3144966671</v>
+        <v>200018</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1944,13 +2960,13 @@
         <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D66">
-        <v>2020019</v>
+        <v>200019</v>
       </c>
       <c r="E66">
-        <v>3132435826</v>
+        <v>200019</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1961,13 +2977,13 @@
         <v>73</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D67">
-        <v>2020020</v>
+        <v>220013</v>
       </c>
       <c r="E67">
-        <v>3139445252</v>
+        <v>220013</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1981,10 +2997,10 @@
         <v>7</v>
       </c>
       <c r="D68">
-        <v>2019001</v>
+        <v>190001</v>
       </c>
       <c r="E68">
-        <v>3123995445</v>
+        <v>190001</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1995,13 +3011,13 @@
         <v>75</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D69">
-        <v>2019002</v>
+        <v>190002</v>
       </c>
       <c r="E69">
-        <v>3122557284</v>
+        <v>190002</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2015,10 +3031,10 @@
         <v>7</v>
       </c>
       <c r="D70">
-        <v>2019003</v>
+        <v>190003</v>
       </c>
       <c r="E70">
-        <v>3139656061</v>
+        <v>190003</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2032,10 +3048,10 @@
         <v>7</v>
       </c>
       <c r="D71">
-        <v>2019004</v>
+        <v>190004</v>
       </c>
       <c r="E71">
-        <v>3146179753</v>
+        <v>190004</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2049,10 +3065,10 @@
         <v>7</v>
       </c>
       <c r="D72">
-        <v>2019005</v>
+        <v>190005</v>
       </c>
       <c r="E72">
-        <v>133815098</v>
+        <v>190005</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2066,10 +3082,10 @@
         <v>7</v>
       </c>
       <c r="D73">
-        <v>2019006</v>
+        <v>190006</v>
       </c>
       <c r="E73">
-        <v>3120869236</v>
+        <v>190006</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2080,13 +3096,13 @@
         <v>80</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D74">
-        <v>2019007</v>
+        <v>190007</v>
       </c>
       <c r="E74">
-        <v>139205975</v>
+        <v>190007</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2100,10 +3116,10 @@
         <v>7</v>
       </c>
       <c r="D75">
-        <v>2019008</v>
+        <v>190008</v>
       </c>
       <c r="E75">
-        <v>135058669</v>
+        <v>190008</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2114,13 +3130,13 @@
         <v>82</v>
       </c>
       <c r="C76" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D76">
-        <v>2019009</v>
+        <v>190009</v>
       </c>
       <c r="E76">
-        <v>3124396815</v>
+        <v>190009</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2131,13 +3147,13 @@
         <v>83</v>
       </c>
       <c r="C77" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D77">
-        <v>2019010</v>
+        <v>190010</v>
       </c>
       <c r="E77">
-        <v>3124931342</v>
+        <v>190010</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2148,13 +3164,13 @@
         <v>84</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D78">
-        <v>2019011</v>
+        <v>190011</v>
       </c>
       <c r="E78">
-        <v>3132728862</v>
+        <v>190011</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2168,10 +3184,10 @@
         <v>7</v>
       </c>
       <c r="D79">
-        <v>2019012</v>
+        <v>190012</v>
       </c>
       <c r="E79">
-        <v>3121127806</v>
+        <v>190012</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2185,10 +3201,10 @@
         <v>7</v>
       </c>
       <c r="D80">
-        <v>2019013</v>
+        <v>190013</v>
       </c>
       <c r="E80">
-        <v>3138497283</v>
+        <v>190013</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2202,10 +3218,10 @@
         <v>7</v>
       </c>
       <c r="D81">
-        <v>2019014</v>
+        <v>190014</v>
       </c>
       <c r="E81">
-        <v>126297412</v>
+        <v>190014</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2216,13 +3232,13 @@
         <v>88</v>
       </c>
       <c r="C82" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D82">
-        <v>2019015</v>
+        <v>190015</v>
       </c>
       <c r="E82">
-        <v>3123168446</v>
+        <v>190015</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2236,10 +3252,10 @@
         <v>7</v>
       </c>
       <c r="D83">
-        <v>2019016</v>
+        <v>190016</v>
       </c>
       <c r="E83">
-        <v>3123500447</v>
+        <v>190016</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2253,10 +3269,10 @@
         <v>7</v>
       </c>
       <c r="D84">
-        <v>2019017</v>
+        <v>190017</v>
       </c>
       <c r="E84">
-        <v>3120305177</v>
+        <v>190017</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2267,13 +3283,13 @@
         <v>91</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D85">
-        <v>2019018</v>
+        <v>190018</v>
       </c>
       <c r="E85">
-        <v>3132322587</v>
+        <v>190018</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2284,13 +3300,13 @@
         <v>92</v>
       </c>
       <c r="C86" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D86">
-        <v>2019019</v>
+        <v>220014</v>
       </c>
       <c r="E86">
-        <v>3129624621</v>
+        <v>220014</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2304,10 +3320,10 @@
         <v>7</v>
       </c>
       <c r="D87">
-        <v>2018001</v>
+        <v>180001</v>
       </c>
       <c r="E87">
-        <v>3111502368</v>
+        <v>180001</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2321,10 +3337,10 @@
         <v>7</v>
       </c>
       <c r="D88">
-        <v>2018002</v>
+        <v>180002</v>
       </c>
       <c r="E88">
-        <v>3125522814</v>
+        <v>180002</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2338,10 +3354,10 @@
         <v>7</v>
       </c>
       <c r="D89">
-        <v>2018003</v>
+        <v>180003</v>
       </c>
       <c r="E89">
-        <v>128645248</v>
+        <v>180003</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2352,13 +3368,13 @@
         <v>96</v>
       </c>
       <c r="C90" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D90">
-        <v>2018004</v>
+        <v>180004</v>
       </c>
       <c r="E90">
-        <v>128062854</v>
+        <v>180004</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2372,10 +3388,10 @@
         <v>7</v>
       </c>
       <c r="D91">
-        <v>2018005</v>
+        <v>180005</v>
       </c>
       <c r="E91">
-        <v>3118076459</v>
+        <v>180005</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2389,10 +3405,10 @@
         <v>7</v>
       </c>
       <c r="D92">
-        <v>2018006</v>
+        <v>180006</v>
       </c>
       <c r="E92">
-        <v>3113505201</v>
+        <v>180006</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2406,10 +3422,10 @@
         <v>7</v>
       </c>
       <c r="D93">
-        <v>2018007</v>
+        <v>180007</v>
       </c>
       <c r="E93">
-        <v>3116780589</v>
+        <v>180007</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2423,10 +3439,10 @@
         <v>7</v>
       </c>
       <c r="D94">
-        <v>2018008</v>
+        <v>180008</v>
       </c>
       <c r="E94">
-        <v>3114599103</v>
+        <v>180008</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2440,10 +3456,10 @@
         <v>7</v>
       </c>
       <c r="D95">
-        <v>2018009</v>
+        <v>180009</v>
       </c>
       <c r="E95">
-        <v>3125581676</v>
+        <v>180009</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2457,10 +3473,10 @@
         <v>7</v>
       </c>
       <c r="D96">
-        <v>2018010</v>
+        <v>180010</v>
       </c>
       <c r="E96">
-        <v>3112254211</v>
+        <v>180010</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2474,10 +3490,10 @@
         <v>7</v>
       </c>
       <c r="D97">
-        <v>2018011</v>
+        <v>180011</v>
       </c>
       <c r="E97">
-        <v>3112706593</v>
+        <v>180011</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2491,10 +3507,10 @@
         <v>7</v>
       </c>
       <c r="D98">
-        <v>2018012</v>
+        <v>180012</v>
       </c>
       <c r="E98">
-        <v>3128079011</v>
+        <v>180012</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2508,10 +3524,10 @@
         <v>7</v>
       </c>
       <c r="D99">
-        <v>2018013</v>
+        <v>180013</v>
       </c>
       <c r="E99">
-        <v>3124689706</v>
+        <v>180013</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2525,10 +3541,10 @@
         <v>7</v>
       </c>
       <c r="D100">
-        <v>2018014</v>
+        <v>180014</v>
       </c>
       <c r="E100">
-        <v>3124419517</v>
+        <v>180014</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2539,13 +3555,13 @@
         <v>107</v>
       </c>
       <c r="C101" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D101">
-        <v>2018015</v>
+        <v>180015</v>
       </c>
       <c r="E101">
-        <v>3110002173</v>
+        <v>180015</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2559,10 +3575,10 @@
         <v>7</v>
       </c>
       <c r="D102">
-        <v>2018016</v>
+        <v>180016</v>
       </c>
       <c r="E102">
-        <v>3115192201</v>
+        <v>180016</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2576,10 +3592,10 @@
         <v>7</v>
       </c>
       <c r="D103">
-        <v>2018017</v>
+        <v>180017</v>
       </c>
       <c r="E103">
-        <v>3116058300</v>
+        <v>180017</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2593,10 +3609,10 @@
         <v>7</v>
       </c>
       <c r="D104">
-        <v>2018018</v>
+        <v>180018</v>
       </c>
       <c r="E104">
-        <v>3114451937</v>
+        <v>180018</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2610,10 +3626,10 @@
         <v>7</v>
       </c>
       <c r="D105">
-        <v>2018019</v>
+        <v>180019</v>
       </c>
       <c r="E105">
-        <v>3111393009</v>
+        <v>180019</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2627,10 +3643,10 @@
         <v>7</v>
       </c>
       <c r="D106">
-        <v>2018020</v>
+        <v>180020</v>
       </c>
       <c r="E106">
-        <v>3126042189</v>
+        <v>180020</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2644,10 +3660,10 @@
         <v>7</v>
       </c>
       <c r="D107">
-        <v>2018021</v>
+        <v>180021</v>
       </c>
       <c r="E107">
-        <v>3125514572</v>
+        <v>180021</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2661,10 +3677,10 @@
         <v>7</v>
       </c>
       <c r="D108">
-        <v>2018022</v>
+        <v>180022</v>
       </c>
       <c r="E108">
-        <v>3114041729</v>
+        <v>180022</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2678,10 +3694,10 @@
         <v>7</v>
       </c>
       <c r="D109">
-        <v>2018023</v>
+        <v>180023</v>
       </c>
       <c r="E109">
-        <v>3118701314</v>
+        <v>180023</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2695,10 +3711,10 @@
         <v>7</v>
       </c>
       <c r="D110">
-        <v>2018024</v>
+        <v>180024</v>
       </c>
       <c r="E110">
-        <v>3112121591</v>
+        <v>180024</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2709,13 +3725,13 @@
         <v>117</v>
       </c>
       <c r="C111" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D111">
-        <v>2018025</v>
+        <v>180025</v>
       </c>
       <c r="E111">
-        <v>3126099475</v>
+        <v>180025</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2729,10 +3745,10 @@
         <v>7</v>
       </c>
       <c r="D112">
-        <v>2018026</v>
+        <v>180026</v>
       </c>
       <c r="E112">
-        <v>3127918200</v>
+        <v>180026</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2746,10 +3762,10 @@
         <v>7</v>
       </c>
       <c r="D113">
-        <v>2018027</v>
+        <v>180027</v>
       </c>
       <c r="E113">
-        <v>3127557019</v>
+        <v>180027</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2760,13 +3776,13 @@
         <v>120</v>
       </c>
       <c r="C114" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D114">
-        <v>2018028</v>
+        <v>180028</v>
       </c>
       <c r="E114">
-        <v>126264888</v>
+        <v>180028</v>
       </c>
     </row>
   </sheetData>
@@ -2808,7 +3824,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>122</v>
@@ -2816,7 +3832,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>123</v>
@@ -2824,7 +3840,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>124</v>
@@ -2832,7 +3848,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>125</v>
@@ -2840,7 +3856,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>126</v>
@@ -2848,7 +3864,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>127</v>
@@ -2856,7 +3872,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>128</v>
@@ -2864,7 +3880,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>129</v>

</xml_diff>